<commit_message>
add some (better) NDRange implementations
</commit_message>
<xml_diff>
--- a/KM/KM_data.xlsx
+++ b/KM/KM_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="380">
   <si>
     <t>ALUTs</t>
   </si>
@@ -1321,6 +1321,52 @@
   <si>
     <t>failed</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>private_transpose_uli8_ulo8_simd2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>162,458 / 427,200 ( 38 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>268 / 1,518 ( 18 % )</t>
+  </si>
+  <si>
+    <t>1,123 / 2,713 ( 41 % )</t>
+  </si>
+  <si>
+    <t>private_transpose_uli8_ulo8_simd2_cu2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>261,325 / 427,200 ( 61 % )</t>
+  </si>
+  <si>
+    <t>536 / 1,518 ( 35 % )</t>
+  </si>
+  <si>
+    <t>19,605,896 / 55,562,240 ( 35 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,435 / 2,713 ( 90 % )</t>
+  </si>
+  <si>
+    <t>private_transpose_uli8_ulo8_simd4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>257,029 / 427,200 ( 60 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,894,856 / 55,562,240 ( 32 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,367 / 2,713 ( 87 % )</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1491,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1516,6 +1562,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1798,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2539,7 +2588,7 @@
         <v>77.881</v>
       </c>
       <c r="K21" s="16">
-        <f t="shared" ref="K21:K29" si="1">MMULT(I21,J21)*1000</f>
+        <f t="shared" ref="K21:K32" si="1">MMULT(I21,J21)*1000</f>
         <v>26284837.5</v>
       </c>
     </row>
@@ -2795,1816 +2844,1924 @@
         <v>204208.33333308197</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>238149</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="8">
         <v>599374</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="20">
         <v>250</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="3">
         <v>0.747</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="16">
         <f t="shared" si="1"/>
         <v>186750</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="16"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="16"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="16"/>
-    </row>
-    <row r="33" spans="1:12" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
+    <row r="30" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C30" s="3">
+        <v>161920</v>
+      </c>
+      <c r="D30" s="8">
+        <v>400519</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="I30" s="20">
+        <v>260.41666666700002</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="K30" s="16">
+        <f t="shared" si="1"/>
+        <v>250260.416666987</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C31" s="4">
+        <v>243160</v>
+      </c>
+      <c r="D31" s="14">
+        <v>716016</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="I31" s="9">
+        <v>256.25</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="1"/>
+        <v>148881.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C32" s="3">
+        <v>260284</v>
+      </c>
+      <c r="D32" s="8">
+        <v>684859</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="I32" s="20">
+        <v>194.444444444</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="K32" s="16">
+        <f t="shared" si="1"/>
+        <v>136694.44444413198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B36" s="4">
         <v>14</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="2"/>
-      <c r="K33" s="16"/>
-    </row>
-    <row r="34" spans="1:12" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="2"/>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A37" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="I37" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J37" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K37" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
+    <row r="38" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3">
         <v>59239</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D38" s="8">
         <v>76146</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I35" s="20">
+      <c r="I38" s="20">
         <v>342.5</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J38" s="3">
         <v>86.301000000000002</v>
       </c>
-      <c r="K35" s="16">
-        <f>MMULT(I35,J35)*1000</f>
+      <c r="K38" s="16">
+        <f>MMULT(I38,J38)*1000</f>
         <v>29558092.500000004</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A36" s="3" t="s">
+    <row r="39" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A39" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3">
         <v>61094</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D39" s="8">
         <v>85818</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I36" s="20">
+      <c r="I39" s="20">
         <v>263.88888888899999</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J39" s="3">
         <v>37.414999999999999</v>
       </c>
-      <c r="K36" s="16">
-        <f>MMULT(I36,J36)*1000</f>
+      <c r="K39" s="16">
+        <f>MMULT(I39,J39)*1000</f>
         <v>9873402.7777819335</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A37" s="3" t="s">
+    <row r="40" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A40" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C40" s="3">
         <v>64342</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D40" s="8">
         <v>92181</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I37" s="20">
+      <c r="I40" s="20">
         <v>290</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J40" s="3">
         <v>34.106000000000002</v>
       </c>
-      <c r="K37" s="16">
-        <f t="shared" ref="K37:K49" si="2">MMULT(I37,J37)*1000</f>
+      <c r="K40" s="16">
+        <f t="shared" ref="K40:K52" si="2">MMULT(I40,J40)*1000</f>
         <v>9890740</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
+    <row r="41" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A41" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C41" s="3">
         <v>64334</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D41" s="8">
         <v>91946</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I38" s="20">
+      <c r="I41" s="20">
         <v>306.25</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J41" s="3">
         <v>32.271000000000001</v>
       </c>
-      <c r="K38" s="16">
+      <c r="K41" s="16">
         <f t="shared" si="2"/>
         <v>9882993.75</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A39" s="3" t="s">
+    <row r="42" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A42" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C42" s="3">
         <v>66891</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D42" s="8">
         <v>95959</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I39" s="20">
+      <c r="I42" s="20">
         <v>271.875</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J42" s="3">
         <v>36.344000000000001</v>
       </c>
-      <c r="K39" s="16">
+      <c r="K42" s="16">
         <f t="shared" si="2"/>
         <v>9881025</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="3" t="s">
+    <row r="43" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A43" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C43" s="3">
         <v>65770</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D43" s="8">
         <v>96290</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="I40" s="20">
+      <c r="I43" s="20">
         <v>297.5</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J43" s="3">
         <v>33.229999999999997</v>
       </c>
-      <c r="K40" s="16">
+      <c r="K43" s="16">
         <f t="shared" si="2"/>
         <v>9885925</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A41" s="3" t="s">
+    <row r="44" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A44" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C44" s="3">
         <v>61941</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D44" s="8">
         <v>88976</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I41" s="20">
+      <c r="I44" s="20">
         <v>315</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J44" s="3">
         <v>31.375</v>
       </c>
-      <c r="K41" s="16">
+      <c r="K44" s="16">
         <f t="shared" si="2"/>
         <v>9883125</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
-      <c r="A42" s="3" t="s">
+    <row r="45" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C45" s="3">
         <v>68892</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D45" s="8">
         <v>97257</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="I42" s="20">
+      <c r="I45" s="20">
         <v>302.5</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J45" s="3">
         <v>32.661000000000001</v>
       </c>
-      <c r="K42" s="16">
+      <c r="K45" s="16">
         <f t="shared" si="2"/>
         <v>9879952.5000000019</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.15">
-      <c r="A43" s="3" t="s">
+    <row r="46" spans="1:11" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.15">
+      <c r="A46" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C46" s="3">
         <v>72638</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D46" s="8">
         <v>112599</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I43" s="20">
+      <c r="I46" s="20">
         <v>265.625</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J46" s="3">
         <v>37.173000000000002</v>
       </c>
-      <c r="K43" s="16">
+      <c r="K46" s="16">
         <f t="shared" si="2"/>
         <v>9874078.125</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
+    <row r="47" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+      <c r="A47" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C47" s="3">
         <v>71176</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D47" s="8">
         <v>106155</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="I44" s="20">
+      <c r="I47" s="20">
         <v>284.375</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J47" s="3">
         <v>17.454999999999998</v>
       </c>
-      <c r="K44" s="16">
+      <c r="K47" s="16">
         <f t="shared" si="2"/>
         <v>4963765.6249999991</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A45" s="4" t="s">
+    <row r="48" spans="1:11" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A48" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C48" s="4">
         <v>86588</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D48" s="14">
         <v>136432</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="H48" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="I45" s="9">
+      <c r="I48" s="9">
         <v>255.555555556</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J48" s="4">
         <v>9.7910000000000004</v>
       </c>
-      <c r="K45" s="5">
+      <c r="K48" s="5">
         <f t="shared" si="2"/>
         <v>2502144.4444487961</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A46" s="3" t="s">
+    <row r="49" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C49" s="3">
         <v>117130</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D49" s="8">
         <v>200217</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I46" s="20">
+      <c r="I49" s="20">
         <v>243.75</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J49" s="3">
         <v>5.1689999999999996</v>
       </c>
-      <c r="K46" s="16">
+      <c r="K49" s="16">
         <f t="shared" si="2"/>
         <v>1259943.75</v>
       </c>
-      <c r="L46" s="12" t="s">
+      <c r="L49" s="12" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A47" s="3" t="s">
+    <row r="50" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A50" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C50" s="3">
         <v>168977</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D50" s="8">
         <v>318108</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="I47" s="20">
+      <c r="I50" s="20">
         <v>247.222222222</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J50" s="3">
         <v>2.617</v>
       </c>
-      <c r="K47" s="16">
+      <c r="K50" s="16">
         <f t="shared" si="2"/>
         <v>646980.55555497401</v>
       </c>
-      <c r="L47" s="12" t="s">
+      <c r="L50" s="12" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A48" s="3" t="s">
+    <row r="51" spans="1:12" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C51" s="3">
         <v>72737</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D51" s="8">
         <v>104844</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I48" s="20">
+      <c r="I51" s="20">
         <v>233.333333334</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J51" s="3">
         <v>1098.2639999999999</v>
       </c>
-      <c r="K48" s="16">
+      <c r="K51" s="16">
         <f t="shared" si="2"/>
         <v>256261600.00073215</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="16" t="e">
+    <row r="52" spans="1:12" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="16"/>
-    </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="16"/>
-    </row>
-    <row r="52" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A52" s="4" t="s">
+    <row r="53" spans="1:12" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="16"/>
+    </row>
+    <row r="54" spans="1:12" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="1:12" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A55" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B55" s="4">
         <v>12</v>
       </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="2"/>
-      <c r="K52" s="16"/>
-    </row>
-    <row r="53" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A53" s="6" t="s">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="2"/>
+      <c r="K55" s="16"/>
+    </row>
+    <row r="56" spans="1:12" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A56" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B56" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G56" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H53" s="7" t="s">
+      <c r="H56" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I56" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J53" s="18" t="s">
+      <c r="J56" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K53" s="19" t="s">
+      <c r="K56" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="13" t="s">
+    <row r="57" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C57" s="3">
         <v>61115</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D57" s="8">
         <v>79769</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="I54" s="20">
+      <c r="I57" s="20">
         <v>337.5</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J57" s="3">
         <v>77.847999999999999</v>
       </c>
-      <c r="K54" s="16">
-        <f t="shared" ref="K54:K65" si="3">MMULT(I54,J54)*1000</f>
+      <c r="K57" s="16">
+        <f t="shared" ref="K57:K68" si="3">MMULT(I57,J57)*1000</f>
         <v>26273700</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="3" t="s">
+    <row r="58" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C58" s="3">
         <v>62008</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D58" s="8">
         <v>80932</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="I55" s="20">
+      <c r="I58" s="20">
         <v>360</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J58" s="3">
         <v>72.984999999999999</v>
       </c>
-      <c r="K55" s="16">
+      <c r="K58" s="16">
         <f t="shared" si="3"/>
         <v>26274600</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="3" t="s">
+    <row r="59" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B59" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C59" s="8">
         <v>64984</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D59" s="8">
         <v>86624</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H59" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="I56" s="20">
+      <c r="I59" s="20">
         <v>343.75</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J59" s="3">
         <v>38.363</v>
       </c>
-      <c r="K56" s="16">
+      <c r="K59" s="16">
         <f t="shared" si="3"/>
         <v>13187281.25</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="3" t="s">
+    <row r="60" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C60" s="3">
         <v>67326</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D60" s="8">
         <v>107031</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="I57" s="20">
+      <c r="I60" s="20">
         <v>285</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J60" s="3">
         <v>5.9740000000000002</v>
       </c>
-      <c r="K57" s="16">
+      <c r="K60" s="16">
         <f t="shared" si="3"/>
         <v>1702590.0000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="3" t="s">
+    <row r="61" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C61" s="3">
         <v>66020</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D61" s="8">
         <v>105345</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I58" s="20">
+      <c r="I61" s="20">
         <v>285</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J61" s="3">
         <v>5.9729999999999999</v>
       </c>
-      <c r="K58" s="16">
+      <c r="K61" s="16">
         <f t="shared" si="3"/>
         <v>1702305</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="3" t="s">
+    <row r="62" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C62" s="3">
         <v>62903</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D62" s="8">
         <v>97700</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I59" s="20">
+      <c r="I62" s="20">
         <v>287.5</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J62" s="3">
         <v>5.8760000000000003</v>
       </c>
-      <c r="K59" s="16">
+      <c r="K62" s="16">
         <f t="shared" si="3"/>
         <v>1689350.0000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="3" t="s">
+    <row r="63" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C63" s="3">
         <v>61638</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D63" s="8">
         <v>95718</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H63" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="I60" s="20">
+      <c r="I63" s="20">
         <v>290.625</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J63" s="3">
         <v>5.8220000000000001</v>
       </c>
-      <c r="K60" s="16">
+      <c r="K63" s="16">
         <f t="shared" si="3"/>
         <v>1692018.75</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="3" t="s">
+    <row r="64" spans="1:12" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C64" s="3">
         <v>190075</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D64" s="8">
         <v>429192</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G64" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H64" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="I61" s="20">
+      <c r="I64" s="20">
         <v>275</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J64" s="3">
         <v>0.95</v>
       </c>
-      <c r="K61" s="16">
+      <c r="K64" s="16">
         <f t="shared" si="3"/>
         <v>261250</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="3" t="s">
+    <row r="65" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A65" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C65" s="3">
         <v>244623</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D65" s="8">
         <v>620250</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H65" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="I62" s="20">
+      <c r="I65" s="20">
         <v>256.25</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J65" s="3">
         <v>0.76200000000000001</v>
       </c>
-      <c r="K62" s="16">
+      <c r="K65" s="16">
         <f t="shared" si="3"/>
         <v>195262.5</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A63" s="3" t="s">
+    <row r="66" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A66" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C66" s="3">
         <v>245850</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D66" s="8">
         <v>621931</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="I63" s="20">
+      <c r="I66" s="20">
         <v>280</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J66" s="3">
         <v>0.72099999999999997</v>
       </c>
-      <c r="K63" s="16">
-        <f>MMULT(I63,J63)*1000</f>
+      <c r="K66" s="16">
+        <f>MMULT(I66,J66)*1000</f>
         <v>201880</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A64" s="3" t="s">
+    <row r="67" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A67" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C67" s="3">
         <v>218265</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D67" s="8">
         <v>527068</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F67" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="I64" s="20">
+      <c r="I67" s="20">
         <v>285</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J67" s="3">
         <v>0.68700000000000006</v>
       </c>
-      <c r="K64" s="16">
+      <c r="K67" s="16">
         <f t="shared" si="3"/>
         <v>195795.00000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A65" s="4" t="s">
+    <row r="68" spans="1:11" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A68" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C68" s="4">
         <v>269040</v>
       </c>
-      <c r="D65" s="14">
+      <c r="D68" s="14">
         <v>694873</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F68" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G68" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="H65" s="4" t="s">
+      <c r="H68" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="I65" s="9">
+      <c r="I68" s="9">
         <v>254.166666666</v>
       </c>
-      <c r="J65" s="4">
+      <c r="J68" s="4">
         <v>0.629</v>
       </c>
-      <c r="K65" s="5">
+      <c r="K68" s="5">
         <f t="shared" si="3"/>
         <v>159870.83333291402</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A69" s="4" t="s">
+    <row r="72" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A72" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B72" s="4">
         <v>17</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="2"/>
-      <c r="K69" s="16"/>
-    </row>
-    <row r="70" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A70" s="6" t="s">
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="2"/>
+      <c r="K72" s="16"/>
+    </row>
+    <row r="73" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A73" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B73" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C73" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D73" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E73" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F73" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="G73" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H70" s="7" t="s">
+      <c r="H73" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I70" s="17" t="s">
+      <c r="I73" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J70" s="18" t="s">
+      <c r="J73" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K70" s="19" t="s">
+      <c r="K73" s="19" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C71" s="3">
-        <v>61087</v>
-      </c>
-      <c r="D71" s="8">
-        <v>78196</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I71" s="20">
-        <v>345.83333333299998</v>
-      </c>
-      <c r="J71" s="3">
-        <v>85.472999999999999</v>
-      </c>
-      <c r="K71" s="16">
-        <f>MMULT(I71,J71)*1000</f>
-        <v>29559412.499971505</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A72" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C72" s="3">
-        <v>63012</v>
-      </c>
-      <c r="D72" s="8">
-        <v>87895</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I72" s="20">
-        <v>261.66666666700002</v>
-      </c>
-      <c r="J72" s="3">
-        <v>37.796999999999997</v>
-      </c>
-      <c r="K72" s="16">
-        <f>MMULT(I72,J72)*1000</f>
-        <v>9890215.0000125989</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A73" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C73" s="3">
-        <v>62477</v>
-      </c>
-      <c r="D73" s="8">
-        <v>80365</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I73" s="20">
-        <v>297.5</v>
-      </c>
-      <c r="J73" s="3">
-        <v>49.831000000000003</v>
-      </c>
-      <c r="K73" s="16">
-        <f t="shared" ref="K73:K87" si="4">MMULT(I73,J73)*1000</f>
-        <v>14824722.500000002</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C74" s="3">
+        <v>61087</v>
+      </c>
+      <c r="D74" s="8">
+        <v>78196</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I74" s="20">
+        <v>345.83333333299998</v>
+      </c>
+      <c r="J74" s="3">
+        <v>85.472999999999999</v>
+      </c>
+      <c r="K74" s="16">
+        <f>MMULT(I74,J74)*1000</f>
+        <v>29559412.499971505</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A75" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="C75" s="3">
+        <v>63012</v>
+      </c>
+      <c r="D75" s="8">
+        <v>87895</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I75" s="20">
+        <v>261.66666666700002</v>
+      </c>
+      <c r="J75" s="3">
+        <v>37.796999999999997</v>
+      </c>
+      <c r="K75" s="16">
+        <f>MMULT(I75,J75)*1000</f>
+        <v>9890215.0000125989</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A76" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="C76" s="3">
+        <v>62477</v>
+      </c>
+      <c r="D76" s="8">
+        <v>80365</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I76" s="20">
+        <v>297.5</v>
+      </c>
+      <c r="J76" s="3">
+        <v>49.831000000000003</v>
+      </c>
+      <c r="K76" s="16">
+        <f t="shared" ref="K76:K90" si="4">MMULT(I76,J76)*1000</f>
+        <v>14824722.500000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A77" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B77" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C77" s="3">
         <v>76726</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D77" s="8">
         <v>101501</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F77" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="H77" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="I74" s="20">
+      <c r="I77" s="20">
         <v>300</v>
       </c>
-      <c r="J74" s="3">
+      <c r="J77" s="3">
         <v>24.914000000000001</v>
       </c>
-      <c r="K74" s="16">
+      <c r="K77" s="16">
         <f t="shared" si="4"/>
         <v>7474200.0000000009</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A75" s="3" t="s">
+    <row r="78" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A78" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B78" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C78" s="3">
         <v>107967</v>
       </c>
-      <c r="D75" s="8">
+      <c r="D78" s="8">
         <v>174685</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H78" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I75" s="20">
+      <c r="I78" s="20">
         <v>232.5</v>
       </c>
-      <c r="J75" s="3">
+      <c r="J78" s="3">
         <v>10.893000000000001</v>
       </c>
-      <c r="K75" s="16">
+      <c r="K78" s="16">
         <f t="shared" si="4"/>
         <v>2532622.5</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
+    <row r="79" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A79" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C79" s="3">
         <v>98193</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D79" s="8">
         <v>165605</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="F79" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G76" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="H79" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="I76" s="20">
+      <c r="I79" s="20">
         <v>259.375</v>
       </c>
-      <c r="J76" s="3">
+      <c r="J79" s="3">
         <v>9.8059999999999992</v>
       </c>
-      <c r="K76" s="16">
+      <c r="K79" s="16">
         <f t="shared" si="4"/>
         <v>2543431.2499999995</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A77" s="3" t="s">
+    <row r="80" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A80" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C80" s="3">
         <v>105514</v>
       </c>
-      <c r="D77" s="8">
+      <c r="D80" s="8">
         <v>143938</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E80" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F80" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G80" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="H80" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="I77" s="20">
+      <c r="I80" s="20">
         <v>290.625</v>
       </c>
-      <c r="J77" s="3">
+      <c r="J80" s="3">
         <v>13.157999999999999</v>
       </c>
-      <c r="K77" s="16">
+      <c r="K80" s="16">
         <f t="shared" si="4"/>
         <v>3824043.75</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A78" s="3" t="s">
+    <row r="81" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A81" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B81" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C81" s="3">
         <v>163349</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D81" s="8">
         <v>229409</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="F81" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G81" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H78" s="3" t="s">
+      <c r="H81" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="I78" s="20">
+      <c r="I81" s="20">
         <v>250</v>
       </c>
-      <c r="J78" s="3">
+      <c r="J81" s="3">
         <v>67.367999999999995</v>
       </c>
-      <c r="K78" s="16">
+      <c r="K81" s="16">
         <f t="shared" si="4"/>
         <v>16842000</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A79" s="3" t="s">
+    <row r="82" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A82" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B82" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C82" s="3">
         <v>135660</v>
       </c>
-      <c r="D79" s="8">
+      <c r="D82" s="8">
         <v>216391</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F82" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G82" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="H79" s="3" t="s">
+      <c r="H82" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="I79" s="20">
+      <c r="I82" s="20">
         <v>230.555555556</v>
       </c>
-      <c r="J79" s="3">
+      <c r="J82" s="3">
         <v>37.722000000000001</v>
       </c>
-      <c r="K79" s="16">
+      <c r="K82" s="16">
         <f t="shared" si="4"/>
         <v>8697016.6666834317</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A80" s="3" t="s">
+    <row r="83" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A83" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C83" s="3">
         <v>61467</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D83" s="8">
         <v>77939</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F80" s="3" t="s">
+      <c r="F83" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="H83" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I80" s="20">
+      <c r="I83" s="20">
         <v>312.5</v>
       </c>
-      <c r="J80" s="3">
+      <c r="J83" s="3">
         <v>94.557000000000002</v>
       </c>
-      <c r="K80" s="16">
+      <c r="K83" s="16">
         <f t="shared" si="4"/>
         <v>29549062.5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A81" s="3" t="s">
+    <row r="84" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A84" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C84" s="3">
         <v>76652</v>
       </c>
-      <c r="D81" s="8">
+      <c r="D84" s="8">
         <v>106272</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="F84" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="H84" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I81" s="20">
+      <c r="I84" s="20">
         <v>275</v>
       </c>
-      <c r="J81" s="3">
+      <c r="J84" s="3">
         <v>53.838000000000001</v>
       </c>
-      <c r="K81" s="16">
+      <c r="K84" s="16">
         <f t="shared" si="4"/>
         <v>14805450</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A82" s="3" t="s">
+    <row r="85" spans="1:11" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A85" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C85" s="3">
         <v>67497</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D85" s="8">
         <v>91915</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="F85" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H85" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I82" s="20">
+      <c r="I85" s="20">
         <v>325</v>
       </c>
-      <c r="J82" s="3">
+      <c r="J85" s="3">
         <v>45.59</v>
       </c>
-      <c r="K82" s="16">
-        <f>MMULT(I82,J82)*1000</f>
+      <c r="K85" s="16">
+        <f>MMULT(I85,J85)*1000</f>
         <v>14816750.000000002</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A83" s="3" t="s">
+    <row r="86" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A86" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C86" s="3">
         <v>76256</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D86" s="8">
         <v>105588</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="F86" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="H86" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="I83" s="20">
+      <c r="I86" s="20">
         <v>267.5</v>
       </c>
-      <c r="J83" s="3">
+      <c r="J86" s="3">
         <v>55.344999999999999</v>
       </c>
-      <c r="K83" s="16">
+      <c r="K86" s="16">
         <f t="shared" si="4"/>
         <v>14804787.5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A84" s="3" t="s">
+    <row r="87" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A87" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C87" s="3">
         <v>67323</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D87" s="8">
         <v>91359</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E87" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="F87" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H87" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="I84" s="20">
+      <c r="I87" s="20">
         <v>325</v>
       </c>
-      <c r="J84" s="3">
+      <c r="J87" s="3">
         <v>45.625999999999998</v>
       </c>
-      <c r="K84" s="16">
+      <c r="K87" s="16">
         <f t="shared" si="4"/>
         <v>14828449.999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A85" s="3" t="s">
+    <row r="88" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A88" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C88" s="3">
         <v>94743</v>
       </c>
-      <c r="D85" s="8">
+      <c r="D88" s="8">
         <v>163548</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="F88" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G85" s="3" t="s">
+      <c r="G88" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="H88" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="I85" s="20">
+      <c r="I88" s="20">
         <v>295</v>
       </c>
-      <c r="J85" s="3">
+      <c r="J88" s="3">
         <v>8.6289999999999996</v>
       </c>
-      <c r="K85" s="16">
+      <c r="K88" s="16">
         <f t="shared" si="4"/>
         <v>2545555</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A86" s="3" t="s">
+    <row r="89" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A89" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C89" s="3">
         <v>142626</v>
       </c>
-      <c r="D86" s="8">
+      <c r="D89" s="8">
         <v>269768</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="F89" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G86" s="3" t="s">
+      <c r="G89" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H86" s="3" t="s">
+      <c r="H89" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I86" s="20">
+      <c r="I89" s="20">
         <v>275</v>
       </c>
-      <c r="J86" s="3">
+      <c r="J89" s="3">
         <v>4.915</v>
       </c>
-      <c r="K86" s="16">
+      <c r="K89" s="16">
         <f t="shared" si="4"/>
         <v>1351625</v>
       </c>
     </row>
-    <row r="87" spans="1:11" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A87" s="4" t="s">
+    <row r="90" spans="1:11" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A90" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C90" s="4">
         <v>238928</v>
       </c>
-      <c r="D87" s="14">
+      <c r="D90" s="14">
         <v>481719</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="F87" s="4" t="s">
+      <c r="F90" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G87" s="4" t="s">
+      <c r="G90" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="H87" s="4" t="s">
+      <c r="H90" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="I87" s="9">
+      <c r="I90" s="9">
         <v>267.5</v>
       </c>
-      <c r="J87" s="4">
+      <c r="J90" s="4">
         <v>2.9630000000000001</v>
       </c>
-      <c r="K87" s="5">
+      <c r="K90" s="5">
         <f t="shared" si="4"/>
         <v>792602.50000000012</v>
       </c>

</xml_diff>

<commit_message>
k-means clustering with four execution models
</commit_message>
<xml_diff>
--- a/KM/KM_data.xlsx
+++ b/KM/KM_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="378">
   <si>
     <t>ALUTs</t>
   </si>
@@ -897,10 +897,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>baseline(no_local_private)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>baseline</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -980,7 +976,241 @@
     <t>uli8_ulo4_cu3</t>
   </si>
   <si>
-    <t>private_rm_for</t>
+    <t>use local memory for cluster[128*8]; use private memory for feature[8]; remove unused for-loop; transpose feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>idem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. SWI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. NDRange+Channel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1_transpose</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2_transpose</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2_transpose_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2_transpose_read_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2_transpose_uli8_ulo8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-4_transpose_uli8_ulo6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-2_transpose_uli8_ulo12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kernel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-1_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-4_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer cluster[128*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer cluster[128*8]; use private memory for feature[8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster_1-8_uli4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2stages</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer intermediate value between two stages</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature+cluster_1-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer cluster[128*8] and feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature+cluster_1-2_transpose</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_1-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_1-2_transpose</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_1-4_transpose_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_1-8_transpose_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_1-16_transpose_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>transpose feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>transpose feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>transpose feature[25600*8]; read feature[] continuously in kmeans_in kernel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer cluster[128*8] and feature[25600*8]; transpose feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use channel to transfer feature[25600*8]; transpose feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; transpose feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; adjust on data dependency</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; ul8 manually on cluster[128*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; ul8 manually on feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; transpose feature[25600*8]; ul8 manually on cluster[128*8] and feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; transpose feature[25600*8]; adjust on data dependency; ul8 manually on cluster[128*8] and feature[25600*8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">use private memory for feature[8]; ul8 manually on feature[25600*8]; ul2 manually on the outmost loop, similar to simd2 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for feature[8]; ul8 manually on feature[25600*8]; ul2 on the outmost loop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>162,458 / 427,200 ( 38 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>268 / 1,518 ( 18 % )</t>
+  </si>
+  <si>
+    <t>1,123 / 2,713 ( 41 % )</t>
+  </si>
+  <si>
+    <t>261,325 / 427,200 ( 61 % )</t>
+  </si>
+  <si>
+    <t>536 / 1,518 ( 35 % )</t>
+  </si>
+  <si>
+    <t>19,605,896 / 55,562,240 ( 35 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,435 / 2,713 ( 90 % )</t>
+  </si>
+  <si>
+    <t>257,029 / 427,200 ( 60 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,894,856 / 55,562,240 ( 32 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,367 / 2,713 ( 87 % )</t>
+  </si>
+  <si>
+    <t>baseline_no_lmem</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -988,39 +1218,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>private_uli8_ulo8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_uli8_ulo16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_uli8_ulo20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_uli8_ulo8_cu2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_uli8_ulo12_cu2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose_uli8_ulo8_cu3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose_uli8_ulo12_cu2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use local memory for cluster[128*8]; use private memory for feature[8]; remove unused for-loop; transpose feature[25600*8]</t>
+    <t>use local memory for cluster[128*8]; remove unused for-loop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1028,11 +1230,129 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2. SWI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. NDRange+Channel</t>
+    <t>51,193 / 427,200 ( 12 % )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,875,792 / 55,562,240 ( 5 % )</t>
+  </si>
+  <si>
+    <t>360 / 2,713 ( 13 % )</t>
+  </si>
+  <si>
+    <t>idem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_uli8_ulo8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_uli8_ulo16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_uli8_ulo20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_uli8_ulo8_cu2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_uli8_ulo12_cu2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo12_cu2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo8_cu3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo8_simd2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo8_simd2_cu2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8_ulo8_simd4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_rm+=_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_ulm_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_ulm_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_ulm_12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_transpose_rm+=_ulm_12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_ulm_2_ulo2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_ulm_2_ulo4m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmem_ulm_2_ulo2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1_transpose_uli8_ulo2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1_transpose_read_uli8_ulo2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1_transpose_read_uli8_ulo12_ulo2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-1_transpose_read_uli8_ulo16_ulo2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>idem</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1040,333 +1360,8 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1-1_transpose</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-2_transpose</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-2_transpose_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-2_transpose_read_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-1(2)_transpose_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-1(2)_transpose_read_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-2_transpose_uli8_ulo8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-4_transpose_uli8_ulo6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-2_transpose_uli8_ulo12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-1(2)_transpose_read_uli8_ulo12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-1(2)_transpose_read_uli8_ulo16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kernel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-1_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-4_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-4_private_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer cluster[128*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer cluster[128*8]; use private memory for feature[8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster_1-8_uli4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2stages</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer intermediate value between two stages</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature+cluster_1-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer cluster[128*8] and feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature+cluster_1-2_transpose</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_1-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_1-2_transpose</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_1-4_transpose_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_1-8_transpose_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_1-16_transpose_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>basic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>transpose feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>transpose feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>transpose feature[25600*8]; read feature[] continuously in kmeans_in kernel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer cluster[128*8] and feature[25600*8]; transpose feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use channel to transfer feature[25600*8]; transpose feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_rm+=_uli8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; transpose feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; adjust on data dependency</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; ul8 manually on cluster[128*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_2</t>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; ul8 manually on feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose_ul_manually_12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; transpose feature[25600*8]; ul8 manually on cluster[128*8] and feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose_rm+=_ul_manually_12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; transpose feature[25600*8]; adjust on data dependency; ul8 manually on cluster[128*8] and feature[25600*8]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_2_simd2_manually</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_2_simd4_manually</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_2_simd8_manually</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_2_simd16_manually</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">use private memory for feature[8]; ul8 manually on feature[25600*8]; ul2 manually on the outmost loop, similar to simd2 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_ul_manually_2_ulo2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>use private memory for feature[8]; ul8 manually on feature[25600*8]; ul2 on the outmost loop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Note</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,145 / 427,200 ( 23 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>131 / 1,518 ( 9 % )</t>
-  </si>
-  <si>
-    <t>11,026,256 / 55,562,240 ( 20 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>904 / 2,713 ( 33 % )</t>
-  </si>
-  <si>
-    <t>147,558 / 427,200 ( 35 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>259 / 1,518 ( 17 % )</t>
-  </si>
-  <si>
-    <t>13,725,904 / 55,562,240 ( 25 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,188 / 2,713 ( 44 % )</t>
-  </si>
-  <si>
-    <t>failed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>private_transpose_uli8_ulo8_simd2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>162,458 / 427,200 ( 38 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>268 / 1,518 ( 18 % )</t>
-  </si>
-  <si>
-    <t>1,123 / 2,713 ( 41 % )</t>
-  </si>
-  <si>
-    <t>private_transpose_uli8_ulo8_simd2_cu2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>261,325 / 427,200 ( 61 % )</t>
-  </si>
-  <si>
-    <t>536 / 1,518 ( 35 % )</t>
-  </si>
-  <si>
-    <t>19,605,896 / 55,562,240 ( 35 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2,435 / 2,713 ( 90 % )</t>
-  </si>
-  <si>
-    <t>private_transpose_uli8_ulo8_simd4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>257,029 / 427,200 ( 60 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>17,894,856 / 55,562,240 ( 32 % )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2,367 / 2,713 ( 87 % )</t>
+    <t>cluster_1-4_pmem_uli8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1439,7 +1434,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1476,6 +1471,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1491,7 +1492,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1566,6 +1567,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1847,15 +1851,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.25" customWidth="1"/>
+    <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="7" max="7" width="11.25" customWidth="1"/>
     <col min="9" max="11" width="9" style="21"/>
@@ -1866,7 +1870,7 @@
         <v>258</v>
       </c>
       <c r="B1" s="4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1878,10 +1882,10 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
@@ -1913,7 +1917,7 @@
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="C3" s="3">
         <v>59119</v>
@@ -1946,10 +1950,10 @@
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="C4" s="3">
         <v>60786</v>
@@ -1982,10 +1986,10 @@
     </row>
     <row r="5" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>264</v>
+        <v>341</v>
       </c>
       <c r="C5" s="3">
         <v>59268</v>
@@ -2018,10 +2022,10 @@
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C6" s="3">
         <v>61320</v>
@@ -2054,10 +2058,10 @@
     </row>
     <row r="7" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="3">
         <v>132410</v>
@@ -2090,10 +2094,10 @@
     </row>
     <row r="8" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C8" s="3">
         <v>272369</v>
@@ -2126,10 +2130,10 @@
     </row>
     <row r="9" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C9" s="3">
         <v>154666</v>
@@ -2162,10 +2166,10 @@
     </row>
     <row r="10" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C10" s="3">
         <v>186862</v>
@@ -2198,10 +2202,10 @@
     </row>
     <row r="11" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C11" s="3">
         <v>193960</v>
@@ -2234,10 +2238,10 @@
     </row>
     <row r="12" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" s="3">
         <v>63131</v>
@@ -2270,10 +2274,10 @@
     </row>
     <row r="13" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C13" s="3">
         <v>80744</v>
@@ -2306,10 +2310,10 @@
     </row>
     <row r="14" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C14" s="3">
         <v>97680</v>
@@ -2342,10 +2346,10 @@
     </row>
     <row r="15" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C15" s="3">
         <v>114440</v>
@@ -2378,10 +2382,10 @@
     </row>
     <row r="16" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C16" s="3">
         <v>181769</v>
@@ -2414,10 +2418,10 @@
     </row>
     <row r="17" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17" s="3">
         <v>75562</v>
@@ -2450,10 +2454,10 @@
     </row>
     <row r="18" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18" s="3">
         <v>103983</v>
@@ -2486,10 +2490,10 @@
     </row>
     <row r="19" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C19" s="3">
         <v>146009</v>
@@ -2522,10 +2526,10 @@
     </row>
     <row r="20" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C20" s="3">
         <v>245554</v>
@@ -2558,10 +2562,10 @@
     </row>
     <row r="21" spans="1:11" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>280</v>
+        <v>342</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>281</v>
+        <v>340</v>
       </c>
       <c r="C21" s="3">
         <v>59704</v>
@@ -2588,16 +2592,16 @@
         <v>77.881</v>
       </c>
       <c r="K21" s="16">
-        <f t="shared" ref="K21:K32" si="1">MMULT(I21,J21)*1000</f>
+        <f t="shared" ref="K21:K34" si="1">MMULT(I21,J21)*1000</f>
         <v>26284837.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>282</v>
+        <v>350</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C22" s="3">
         <v>121369</v>
@@ -2630,10 +2634,10 @@
     </row>
     <row r="23" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>284</v>
+        <v>351</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C23" s="3">
         <v>200182</v>
@@ -2666,10 +2670,10 @@
     </row>
     <row r="24" spans="1:11" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C24" s="3">
         <v>230214</v>
@@ -2702,10 +2706,10 @@
     </row>
     <row r="25" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>286</v>
+        <v>353</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C25" s="3">
         <v>196613</v>
@@ -2738,10 +2742,10 @@
     </row>
     <row r="26" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>287</v>
+        <v>354</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C26" s="3">
         <v>252417</v>
@@ -2774,245 +2778,275 @@
     </row>
     <row r="27" spans="1:11" s="10" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>283</v>
+        <v>348</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C27" s="3">
-        <v>121846</v>
+        <v>62095</v>
       </c>
       <c r="D27" s="8">
-        <v>248703</v>
+        <v>88485</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>85</v>
+        <v>344</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>87</v>
+        <v>345</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>88</v>
+        <v>346</v>
       </c>
       <c r="I27" s="20">
-        <v>278.125</v>
+        <v>297.5</v>
       </c>
       <c r="J27" s="3">
-        <v>1.6719999999999999</v>
+        <v>11.212</v>
       </c>
       <c r="K27" s="16">
         <f>MMULT(I27,J27)*1000</f>
+        <v>3335569.9999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="16" t="e">
+        <f>MMULT(I28,J28)*1000</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C29" s="3">
+        <v>121846</v>
+      </c>
+      <c r="D29" s="8">
+        <v>248703</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" s="20">
+        <v>278.125</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="K29" s="16">
+        <f>MMULT(I29,J29)*1000</f>
         <v>465025</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C28" s="3">
+    <row r="30" spans="1:11" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" s="3">
         <v>243206</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D30" s="8">
         <v>616438</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="20">
+      <c r="I30" s="20">
         <v>270.83333333299998</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J30" s="3">
         <v>0.754</v>
       </c>
-      <c r="K28" s="16">
-        <f>MMULT(I28,J28)*1000</f>
+      <c r="K30" s="16">
+        <f>MMULT(I30,J30)*1000</f>
         <v>204208.33333308197</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C29" s="3">
+    <row r="31" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C31" s="3">
         <v>238149</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D31" s="8">
         <v>599374</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I29" s="20">
+      <c r="I31" s="20">
         <v>250</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J31" s="3">
         <v>0.747</v>
       </c>
-      <c r="K29" s="16">
+      <c r="K31" s="16">
         <f t="shared" si="1"/>
         <v>186750</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C30" s="3">
+    <row r="32" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" s="3">
         <v>161920</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D32" s="8">
         <v>400519</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="I30" s="20">
+      <c r="E32" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="I32" s="20">
         <v>260.41666666700002</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J32" s="3">
         <v>0.96099999999999997</v>
       </c>
-      <c r="K30" s="16">
+      <c r="K32" s="16">
         <f t="shared" si="1"/>
         <v>250260.416666987</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A31" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C31" s="4">
+    <row r="33" spans="1:11" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C33" s="4">
         <v>243160</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D33" s="14">
         <v>716016</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="I31" s="9">
+      <c r="E33" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="I33" s="9">
         <v>256.25</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J33" s="4">
         <v>0.58099999999999996</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K33" s="5">
         <f t="shared" si="1"/>
         <v>148881.25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A32" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C32" s="3">
+    <row r="34" spans="1:11" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A34" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C34" s="3">
         <v>260284</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D34" s="8">
         <v>684859</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="E34" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="I32" s="20">
+      <c r="G34" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="I34" s="20">
         <v>194.444444444</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J34" s="3">
         <v>0.70299999999999996</v>
       </c>
-      <c r="K32" s="16">
+      <c r="K34" s="16">
         <f t="shared" si="1"/>
         <v>136694.44444413198</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="16"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="16"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
@@ -3027,532 +3061,480 @@
       <c r="J35" s="3"/>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A36" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="B36" s="4">
-        <v>14</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="2"/>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="3"/>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A37" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="C37" s="7" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" s="4">
+        <v>12</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="2"/>
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A39" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D39" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I37" s="17" t="s">
+      <c r="I39" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J39" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K37" s="19" t="s">
+      <c r="K39" s="19" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3">
-        <v>59239</v>
-      </c>
-      <c r="D38" s="8">
-        <v>76146</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I38" s="20">
-        <v>342.5</v>
-      </c>
-      <c r="J38" s="3">
-        <v>86.301000000000002</v>
-      </c>
-      <c r="K38" s="16">
-        <f>MMULT(I38,J38)*1000</f>
-        <v>29558092.500000004</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A39" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3">
-        <v>61094</v>
-      </c>
-      <c r="D39" s="8">
-        <v>85818</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I39" s="20">
-        <v>263.88888888899999</v>
-      </c>
-      <c r="J39" s="3">
-        <v>37.414999999999999</v>
-      </c>
-      <c r="K39" s="16">
-        <f>MMULT(I39,J39)*1000</f>
-        <v>9873402.7777819335</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>338</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="B40" s="3"/>
       <c r="C40" s="3">
+        <v>59239</v>
+      </c>
+      <c r="D40" s="8">
+        <v>76146</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" s="20">
+        <v>342.5</v>
+      </c>
+      <c r="J40" s="3">
+        <v>86.301000000000002</v>
+      </c>
+      <c r="K40" s="16">
+        <f>MMULT(I40,J40)*1000</f>
+        <v>29558092.500000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A41" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3">
+        <v>61094</v>
+      </c>
+      <c r="D41" s="8">
+        <v>85818</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I41" s="20">
+        <v>263.88888888899999</v>
+      </c>
+      <c r="J41" s="3">
+        <v>37.414999999999999</v>
+      </c>
+      <c r="K41" s="16">
+        <f>MMULT(I41,J41)*1000</f>
+        <v>9873402.7777819335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A42" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C42" s="3">
         <v>64342</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D42" s="8">
         <v>92181</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I40" s="20">
+      <c r="I42" s="20">
         <v>290</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J42" s="3">
         <v>34.106000000000002</v>
       </c>
-      <c r="K40" s="16">
-        <f t="shared" ref="K40:K52" si="2">MMULT(I40,J40)*1000</f>
+      <c r="K42" s="16">
+        <f t="shared" ref="K42:K52" si="2">MMULT(I42,J42)*1000</f>
         <v>9890740</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A41" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="C41" s="3">
+    <row r="43" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A43" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C43" s="3">
         <v>64334</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D43" s="8">
         <v>91946</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I41" s="20">
+      <c r="I43" s="20">
         <v>306.25</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J43" s="3">
         <v>32.271000000000001</v>
       </c>
-      <c r="K41" s="16">
+      <c r="K43" s="16">
         <f t="shared" si="2"/>
         <v>9882993.75</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A42" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="C42" s="3">
-        <v>66891</v>
-      </c>
-      <c r="D42" s="8">
-        <v>95959</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I42" s="20">
-        <v>271.875</v>
-      </c>
-      <c r="J42" s="3">
-        <v>36.344000000000001</v>
-      </c>
-      <c r="K42" s="16">
-        <f t="shared" si="2"/>
-        <v>9881025</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A43" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C43" s="3">
-        <v>65770</v>
-      </c>
-      <c r="D43" s="8">
-        <v>96290</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I43" s="20">
-        <v>297.5</v>
-      </c>
-      <c r="J43" s="3">
-        <v>33.229999999999997</v>
-      </c>
-      <c r="K43" s="16">
-        <f t="shared" si="2"/>
-        <v>9885925</v>
-      </c>
-    </row>
     <row r="44" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="C44" s="3">
-        <v>61941</v>
+        <v>66891</v>
       </c>
       <c r="D44" s="8">
-        <v>88976</v>
+        <v>95959</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="I44" s="20">
-        <v>315</v>
+        <v>271.875</v>
       </c>
       <c r="J44" s="3">
-        <v>31.375</v>
+        <v>36.344000000000001</v>
       </c>
       <c r="K44" s="16">
-        <f t="shared" si="2"/>
-        <v>9883125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+        <f>MMULT(I44,J44)*1000</f>
+        <v>9881025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C45" s="3">
-        <v>68892</v>
+        <v>65770</v>
       </c>
       <c r="D45" s="8">
-        <v>97257</v>
+        <v>96290</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>131</v>
       </c>
       <c r="G45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I45" s="20">
+        <v>297.5</v>
+      </c>
+      <c r="J45" s="3">
+        <v>33.229999999999997</v>
+      </c>
+      <c r="K45" s="16">
+        <f>MMULT(I45,J45)*1000</f>
+        <v>9885925</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A46" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C46" s="3">
+        <v>61941</v>
+      </c>
+      <c r="D46" s="8">
+        <v>88976</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I46" s="20">
+        <v>315</v>
+      </c>
+      <c r="J46" s="3">
+        <v>31.375</v>
+      </c>
+      <c r="K46" s="16">
+        <f>MMULT(I46,J46)*1000</f>
+        <v>9883125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+      <c r="A47" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C47" s="3">
+        <v>68892</v>
+      </c>
+      <c r="D47" s="8">
+        <v>97257</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="I45" s="20">
+      <c r="I47" s="20">
         <v>302.5</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J47" s="3">
         <v>32.661000000000001</v>
       </c>
-      <c r="K45" s="16">
+      <c r="K47" s="16">
         <f t="shared" si="2"/>
         <v>9879952.5000000019</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.15">
-      <c r="A46" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C46" s="3">
+    <row r="48" spans="1:11" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.15">
+      <c r="A48" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C48" s="3">
         <v>72638</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D48" s="8">
         <v>112599</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H48" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I46" s="20">
+      <c r="I48" s="20">
         <v>265.625</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J48" s="3">
         <v>37.173000000000002</v>
       </c>
-      <c r="K46" s="16">
+      <c r="K48" s="16">
         <f t="shared" si="2"/>
         <v>9874078.125</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
-      <c r="A47" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="C47" s="3">
+    <row r="49" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" s="3">
         <v>71176</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D49" s="8">
         <v>106155</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="I47" s="20">
+      <c r="I49" s="20">
         <v>284.375</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J49" s="3">
         <v>17.454999999999998</v>
       </c>
-      <c r="K47" s="16">
+      <c r="K49" s="16">
         <f t="shared" si="2"/>
         <v>4963765.6249999991</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A48" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C48" s="4">
+    <row r="50" spans="1:11" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" s="4">
         <v>86588</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D50" s="14">
         <v>136432</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="I48" s="9">
+      <c r="I50" s="9">
         <v>255.555555556</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J50" s="4">
         <v>9.7910000000000004</v>
       </c>
-      <c r="K48" s="5">
+      <c r="K50" s="5">
         <f t="shared" si="2"/>
         <v>2502144.4444487961</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A49" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C49" s="3">
-        <v>117130</v>
-      </c>
-      <c r="D49" s="8">
-        <v>200217</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="I49" s="20">
-        <v>243.75</v>
-      </c>
-      <c r="J49" s="3">
-        <v>5.1689999999999996</v>
-      </c>
-      <c r="K49" s="16">
-        <f t="shared" si="2"/>
-        <v>1259943.75</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A50" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C50" s="3">
-        <v>168977</v>
-      </c>
-      <c r="D50" s="8">
-        <v>318108</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I50" s="20">
-        <v>247.222222222</v>
-      </c>
-      <c r="J50" s="3">
-        <v>2.617</v>
-      </c>
-      <c r="K50" s="16">
-        <f t="shared" si="2"/>
-        <v>646980.55555497401</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
       <c r="C51" s="3">
         <v>72737</v>
@@ -3583,7 +3565,7 @@
         <v>256261600.00073215</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -3599,7 +3581,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -3612,7 +3594,7 @@
       <c r="J53" s="3"/>
       <c r="K53" s="16"/>
     </row>
-    <row r="54" spans="1:12" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11" s="12" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3625,9 +3607,9 @@
       <c r="J54" s="3"/>
       <c r="K54" s="16"/>
     </row>
-    <row r="55" spans="1:12" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B55" s="4">
         <v>12</v>
@@ -3640,12 +3622,12 @@
       <c r="H55" s="2"/>
       <c r="K55" s="16"/>
     </row>
-    <row r="56" spans="1:12" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>0</v>
@@ -3675,7 +3657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13" t="s">
         <v>219</v>
       </c>
@@ -3704,16 +3686,16 @@
         <v>77.847999999999999</v>
       </c>
       <c r="K57" s="16">
-        <f t="shared" ref="K57:K68" si="3">MMULT(I57,J57)*1000</f>
+        <f t="shared" ref="K57:K60" si="3">MMULT(I57,J57)*1000</f>
         <v>26273700</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="C58" s="3">
         <v>62008</v>
@@ -3744,12 +3726,12 @@
         <v>26274600</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C59" s="8">
         <v>64984</v>
@@ -3780,12 +3762,12 @@
         <v>13187281.25</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C60" s="3">
         <v>67326</v>
@@ -3816,12 +3798,12 @@
         <v>1702590.0000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="C61" s="3">
         <v>66020</v>
@@ -3848,196 +3830,196 @@
         <v>5.9729999999999999</v>
       </c>
       <c r="K61" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="K61:K68" si="4">MMULT(I61,J61)*1000</f>
         <v>1702305</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="C62" s="3">
+        <v>190075</v>
+      </c>
+      <c r="D62" s="8">
+        <v>429192</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I62" s="20">
+        <v>275</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K62" s="16">
+        <f t="shared" si="4"/>
+        <v>261250</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A63" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C63" s="3">
+        <v>245850</v>
+      </c>
+      <c r="D63" s="8">
+        <v>621931</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I63" s="20">
+        <v>280</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="K63" s="16">
+        <f t="shared" si="4"/>
+        <v>201880</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A64" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C64" s="3">
+        <v>244623</v>
+      </c>
+      <c r="D64" s="8">
+        <v>620250</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I64" s="20">
+        <v>256.25</v>
+      </c>
+      <c r="J64" s="3">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="K64" s="16">
+        <f t="shared" si="4"/>
+        <v>195262.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C65" s="3">
         <v>62903</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D65" s="8">
         <v>97700</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H65" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I62" s="20">
+      <c r="I65" s="20">
         <v>287.5</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J65" s="3">
         <v>5.8760000000000003</v>
       </c>
-      <c r="K62" s="16">
-        <f t="shared" si="3"/>
+      <c r="K65" s="16">
+        <f t="shared" si="4"/>
         <v>1689350.0000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="C63" s="3">
+    <row r="66" spans="1:11" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C66" s="3">
         <v>61638</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D66" s="8">
         <v>95718</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="I63" s="20">
+      <c r="I66" s="20">
         <v>290.625</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J66" s="3">
         <v>5.8220000000000001</v>
       </c>
-      <c r="K63" s="16">
-        <f t="shared" si="3"/>
+      <c r="K66" s="16">
+        <f t="shared" si="4"/>
         <v>1692018.75</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="C64" s="3">
-        <v>190075</v>
-      </c>
-      <c r="D64" s="8">
-        <v>429192</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="I64" s="20">
-        <v>275</v>
-      </c>
-      <c r="J64" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="K64" s="16">
-        <f t="shared" si="3"/>
-        <v>261250</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A65" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C65" s="3">
-        <v>244623</v>
-      </c>
-      <c r="D65" s="8">
-        <v>620250</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="I65" s="20">
-        <v>256.25</v>
-      </c>
-      <c r="J65" s="3">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="K65" s="16">
-        <f t="shared" si="3"/>
-        <v>195262.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A66" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C66" s="3">
-        <v>245850</v>
-      </c>
-      <c r="D66" s="8">
-        <v>621931</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="I66" s="20">
-        <v>280</v>
-      </c>
-      <c r="J66" s="3">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="K66" s="16">
-        <f>MMULT(I66,J66)*1000</f>
-        <v>201880</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
-        <v>304</v>
+        <v>373</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>335</v>
+        <v>375</v>
       </c>
       <c r="C67" s="3">
         <v>218265</v>
@@ -4064,16 +4046,16 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="K67" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>195795.00000000003</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="s">
-        <v>305</v>
+        <v>374</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C68" s="4">
         <v>269040</v>
@@ -4100,13 +4082,13 @@
         <v>0.629</v>
       </c>
       <c r="K68" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>159870.83333291402</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="s">
-        <v>294</v>
+        <v>376</v>
       </c>
       <c r="B72" s="4">
         <v>17</v>
@@ -4121,10 +4103,10 @@
     </row>
     <row r="73" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>0</v>
@@ -4156,10 +4138,10 @@
     </row>
     <row r="74" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="C74" s="3">
         <v>61087</v>
@@ -4192,10 +4174,10 @@
     </row>
     <row r="75" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C75" s="3">
         <v>63012</v>
@@ -4228,10 +4210,10 @@
     </row>
     <row r="76" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C76" s="3">
         <v>62477</v>
@@ -4258,16 +4240,16 @@
         <v>49.831000000000003</v>
       </c>
       <c r="K76" s="16">
-        <f t="shared" ref="K76:K90" si="4">MMULT(I76,J76)*1000</f>
+        <f t="shared" ref="K76:K90" si="5">MMULT(I76,J76)*1000</f>
         <v>14824722.500000002</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C77" s="3">
         <v>76726</v>
@@ -4294,16 +4276,16 @@
         <v>24.914000000000001</v>
       </c>
       <c r="K77" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7474200.0000000009</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C78" s="3">
         <v>107967</v>
@@ -4330,16 +4312,16 @@
         <v>10.893000000000001</v>
       </c>
       <c r="K78" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2532622.5</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
-        <v>312</v>
+        <v>377</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="C79" s="3">
         <v>98193</v>
@@ -4366,16 +4348,16 @@
         <v>9.8059999999999992</v>
       </c>
       <c r="K79" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2543431.2499999995</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="C80" s="3">
         <v>105514</v>
@@ -4402,16 +4384,16 @@
         <v>13.157999999999999</v>
       </c>
       <c r="K80" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3824043.75</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C81" s="3">
         <v>163349</v>
@@ -4438,16 +4420,16 @@
         <v>67.367999999999995</v>
       </c>
       <c r="K81" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16842000</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C82" s="3">
         <v>135660</v>
@@ -4474,16 +4456,16 @@
         <v>37.722000000000001</v>
       </c>
       <c r="K82" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8697016.6666834317</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="C83" s="3">
         <v>61467</v>
@@ -4510,16 +4492,16 @@
         <v>94.557000000000002</v>
       </c>
       <c r="K83" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29549062.5</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="C84" s="3">
         <v>76652</v>
@@ -4546,16 +4528,16 @@
         <v>53.838000000000001</v>
       </c>
       <c r="K84" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14805450</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="C85" s="3">
         <v>67497</v>
@@ -4588,10 +4570,10 @@
     </row>
     <row r="86" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="C86" s="3">
         <v>76256</v>
@@ -4618,16 +4600,16 @@
         <v>55.344999999999999</v>
       </c>
       <c r="K86" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14804787.5</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="C87" s="3">
         <v>67323</v>
@@ -4654,16 +4636,16 @@
         <v>45.625999999999998</v>
       </c>
       <c r="K87" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14828449.999999998</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C88" s="3">
         <v>94743</v>
@@ -4690,16 +4672,16 @@
         <v>8.6289999999999996</v>
       </c>
       <c r="K88" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2545555</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C89" s="3">
         <v>142626</v>
@@ -4726,16 +4708,16 @@
         <v>4.915</v>
       </c>
       <c r="K89" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1351625</v>
       </c>
     </row>
     <row r="90" spans="1:11" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A90" s="4" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C90" s="4">
         <v>238928</v>
@@ -4762,7 +4744,7 @@
         <v>2.9630000000000001</v>
       </c>
       <c r="K90" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>792602.50000000012</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update experimantal results for KM
</commit_message>
<xml_diff>
--- a/KM/KM_data.xlsx
+++ b/KM/KM_data.xlsx
@@ -2205,11 +2205,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="488023440"/>
-        <c:axId val="488022880"/>
+        <c:axId val="291625456"/>
+        <c:axId val="291626016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="488023440"/>
+        <c:axId val="291625456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2246,7 +2246,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488022880"/>
+        <c:crossAx val="291626016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2254,7 +2254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488022880"/>
+        <c:axId val="291626016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,7 +2362,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488023440"/>
+        <c:crossAx val="291625456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3422,7 +3422,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
-            <a:t>NDRange</a:t>
+            <a:t>NDR</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
@@ -3527,7 +3527,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1600" baseline="0"/>
-            <a:t>+Channel</a:t>
+            <a:t>+C</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400"/>
         </a:p>
@@ -3628,11 +3628,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
-            <a:t>NDRange+</a:t>
+            <a:t>NDR+</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1600" baseline="0"/>
-            <a:t>Channel</a:t>
+            <a:t>C</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400"/>
         </a:p>
@@ -4260,8 +4260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="C95" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC102" sqref="AC102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5183,7 +5183,7 @@
         <v>194810</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="10" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>371</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>242321354.16697684</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="52.5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>385</v>
       </c>

</xml_diff>